<commit_message>
preenchendo planilha com dados do colaborador admitido
</commit_message>
<xml_diff>
--- a/planilha-agendamento.xlsx
+++ b/planilha-agendamento.xlsx
@@ -5,14 +5,14 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\thayna.silva\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricardo.carvalho\Documents\suno\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17256" windowHeight="5880"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17260" windowHeight="5880"/>
   </bookViews>
   <sheets>
-    <sheet name="Solicitação de Agendamento" sheetId="5" r:id="rId1"/>
+    <sheet name="solicitacao-de-agendamento" sheetId="5" r:id="rId1"/>
     <sheet name="Dados Obrigatórios" sheetId="4" r:id="rId2"/>
     <sheet name="Apoio" sheetId="2" state="hidden" r:id="rId3"/>
   </sheets>
@@ -685,12 +685,6 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -704,6 +698,12 @@
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperlink" xfId="1" builtinId="8"/>
@@ -1080,127 +1080,127 @@
       <selection sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="20.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.44140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.88671875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="20.88671875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.109375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="10.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="43.6640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="10.5546875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="3.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.6328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.90625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.90625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.08984375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="43.6328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.54296875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="3.36328125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="5.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="3.88671875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="18.44140625" customWidth="1"/>
-    <col min="16" max="16" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="13.44140625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="5.90625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="3.90625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.453125" customWidth="1"/>
+    <col min="16" max="16" width="14.6328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="13.453125" bestFit="1" customWidth="1"/>
     <col min="18" max="18" width="7" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="3.109375" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="27.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="3.08984375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="27.6328125" bestFit="1" customWidth="1"/>
     <col min="21" max="21" width="21" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="17.44140625" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="39.109375" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="18.88671875" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="18.6640625" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="23.33203125" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="47.6640625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="25.6640625" hidden="1" customWidth="1"/>
-    <col min="29" max="16383" width="8.88671875" hidden="1"/>
-    <col min="16384" max="16384" width="4.88671875" hidden="1"/>
+    <col min="22" max="22" width="17.453125" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="39.08984375" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="18.6328125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="23.36328125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="47.6328125" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="25.6328125" hidden="1" customWidth="1"/>
+    <col min="29" max="16383" width="8.90625" hidden="1"/>
+    <col min="16384" max="16384" width="4.90625" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="44" customFormat="1" ht="27.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="42" t="s">
+    <row r="1" spans="1:28" s="42" customFormat="1" ht="26" x14ac:dyDescent="0.35">
+      <c r="A1" s="40" t="s">
         <v>50</v>
       </c>
-      <c r="B1" s="42" t="s">
+      <c r="B1" s="40" t="s">
         <v>68</v>
       </c>
-      <c r="C1" s="42" t="s">
+      <c r="C1" s="40" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="42" t="s">
+      <c r="D1" s="40" t="s">
         <v>57</v>
       </c>
-      <c r="E1" s="42" t="s">
+      <c r="E1" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F1" s="42" t="s">
+      <c r="F1" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="42" t="s">
+      <c r="G1" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="H1" s="42" t="s">
+      <c r="H1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="I1" s="42" t="s">
+      <c r="I1" s="40" t="s">
         <v>51</v>
       </c>
-      <c r="J1" s="42" t="s">
+      <c r="J1" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="K1" s="42" t="s">
+      <c r="K1" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="L1" s="42" t="s">
+      <c r="L1" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="M1" s="42" t="s">
+      <c r="M1" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="N1" s="43" t="s">
+      <c r="N1" s="41" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="42" t="s">
+      <c r="O1" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="P1" s="42" t="s">
+      <c r="P1" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="Q1" s="42" t="s">
+      <c r="Q1" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="R1" s="42" t="s">
+      <c r="R1" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="S1" s="42" t="s">
-        <v>0</v>
-      </c>
-      <c r="T1" s="42" t="s">
+      <c r="S1" s="40" t="s">
+        <v>0</v>
+      </c>
+      <c r="T1" s="40" t="s">
         <v>52</v>
       </c>
-      <c r="U1" s="42" t="s">
+      <c r="U1" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="V1" s="42" t="s">
+      <c r="V1" s="40" t="s">
         <v>19</v>
       </c>
-      <c r="W1" s="42" t="s">
+      <c r="W1" s="40" t="s">
         <v>48</v>
       </c>
-      <c r="X1" s="42" t="s">
+      <c r="X1" s="40" t="s">
         <v>49</v>
       </c>
-      <c r="Y1" s="41" t="s">
+      <c r="Y1" s="39" t="s">
         <v>69</v>
       </c>
-      <c r="Z1" s="41" t="s">
+      <c r="Z1" s="39" t="s">
         <v>70</v>
       </c>
-      <c r="AA1" s="41" t="s">
+      <c r="AA1" s="39" t="s">
         <v>71</v>
       </c>
-      <c r="AB1" s="41" t="s">
+      <c r="AB1" s="39" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A2" s="30"/>
       <c r="B2" s="31"/>
       <c r="C2" s="32"/>
@@ -1230,7 +1230,7 @@
       <c r="AA2" s="34"/>
       <c r="AB2" s="34"/>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A3" s="30"/>
       <c r="B3" s="31"/>
       <c r="C3" s="32"/>
@@ -1260,7 +1260,7 @@
       <c r="AA3" s="34"/>
       <c r="AB3" s="34"/>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A4" s="30"/>
       <c r="B4" s="31"/>
       <c r="C4" s="32"/>
@@ -1290,7 +1290,7 @@
       <c r="AA4" s="34"/>
       <c r="AB4" s="34"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A5" s="30"/>
       <c r="B5" s="31"/>
       <c r="C5" s="32"/>
@@ -1320,7 +1320,7 @@
       <c r="AA5" s="34"/>
       <c r="AB5" s="34"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A6" s="30"/>
       <c r="B6" s="31"/>
       <c r="C6" s="32"/>
@@ -1350,7 +1350,7 @@
       <c r="AA6" s="34"/>
       <c r="AB6" s="34"/>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A7" s="30"/>
       <c r="B7" s="31"/>
       <c r="C7" s="32"/>
@@ -1380,7 +1380,7 @@
       <c r="AA7" s="34"/>
       <c r="AB7" s="34"/>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A8" s="30"/>
       <c r="B8" s="31"/>
       <c r="C8" s="32"/>
@@ -1410,7 +1410,7 @@
       <c r="AA8" s="34"/>
       <c r="AB8" s="34"/>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A9" s="30"/>
       <c r="B9" s="31"/>
       <c r="C9" s="32"/>
@@ -1440,7 +1440,7 @@
       <c r="AA9" s="34"/>
       <c r="AB9" s="34"/>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A10" s="30"/>
       <c r="B10" s="31"/>
       <c r="C10" s="32"/>
@@ -1470,7 +1470,7 @@
       <c r="AA10" s="34"/>
       <c r="AB10" s="34"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A11" s="30"/>
       <c r="B11" s="31"/>
       <c r="C11" s="32"/>
@@ -1500,7 +1500,7 @@
       <c r="AA11" s="34"/>
       <c r="AB11" s="34"/>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A12" s="28"/>
       <c r="B12" s="29"/>
       <c r="C12" s="32"/>
@@ -1542,7 +1542,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A13" s="28"/>
       <c r="B13" s="29"/>
       <c r="C13" s="32"/>
@@ -1584,7 +1584,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A14" s="28"/>
       <c r="B14" s="29"/>
       <c r="C14" s="32"/>
@@ -1626,7 +1626,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A15" s="28"/>
       <c r="B15" s="29"/>
       <c r="C15" s="32"/>
@@ -1668,7 +1668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A16" s="28"/>
       <c r="B16" s="29"/>
       <c r="C16" s="32"/>
@@ -1710,7 +1710,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A17" s="28"/>
       <c r="B17" s="29"/>
       <c r="C17" s="32"/>
@@ -1752,7 +1752,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A18" s="28"/>
       <c r="B18" s="29"/>
       <c r="C18" s="32"/>
@@ -1794,7 +1794,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A19" s="28"/>
       <c r="B19" s="29"/>
       <c r="C19" s="32"/>
@@ -1836,7 +1836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A20" s="28"/>
       <c r="B20" s="29"/>
       <c r="C20" s="32"/>
@@ -1878,7 +1878,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.35">
       <c r="A21" s="28"/>
       <c r="B21" s="29"/>
       <c r="C21" s="32"/>
@@ -1970,87 +1970,87 @@
       <selection pane="bottomRight" activeCell="A8" sqref="A8:XFD8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9.08984375" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="15.109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="15.08984375" style="1" customWidth="1"/>
     <col min="2" max="2" width="14" style="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5546875" style="5" customWidth="1"/>
-    <col min="4" max="4" width="11.5546875" style="1" customWidth="1"/>
-    <col min="5" max="6" width="9.109375" style="1"/>
-    <col min="7" max="7" width="15.44140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="9.109375" style="1"/>
-    <col min="9" max="9" width="13.5546875" style="5" bestFit="1" customWidth="1"/>
-    <col min="10" max="19" width="9.109375" style="1"/>
-    <col min="20" max="20" width="15.88671875" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10.44140625" style="1" customWidth="1"/>
-    <col min="22" max="22" width="12.6640625" style="5" customWidth="1"/>
-    <col min="23" max="23" width="12.5546875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="9.54296875" style="5" customWidth="1"/>
+    <col min="4" max="4" width="11.54296875" style="1" customWidth="1"/>
+    <col min="5" max="6" width="9.08984375" style="1"/>
+    <col min="7" max="7" width="15.453125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.08984375" style="1"/>
+    <col min="9" max="9" width="13.54296875" style="5" bestFit="1" customWidth="1"/>
+    <col min="10" max="19" width="9.08984375" style="1"/>
+    <col min="20" max="20" width="15.90625" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10.453125" style="1" customWidth="1"/>
+    <col min="22" max="22" width="12.6328125" style="5" customWidth="1"/>
+    <col min="23" max="23" width="12.54296875" style="1" customWidth="1"/>
     <col min="24" max="24" width="15" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="16384" width="9.109375" style="1"/>
+    <col min="25" max="16384" width="9.08984375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="39" t="s">
+    <row r="1" spans="1:24" s="2" customFormat="1" ht="28.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="43" t="s">
         <v>59</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
-      <c r="M1" s="39"/>
-      <c r="N1" s="39"/>
-      <c r="O1" s="39"/>
-      <c r="P1" s="39"/>
-      <c r="Q1" s="39"/>
-      <c r="R1" s="39"/>
-      <c r="S1" s="39"/>
-      <c r="T1" s="39"/>
-      <c r="U1" s="39"/>
-      <c r="V1" s="39"/>
-      <c r="W1" s="39"/>
-      <c r="X1" s="39"/>
-    </row>
-    <row r="2" spans="1:24" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="40" t="s">
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
+      <c r="H1" s="43"/>
+      <c r="I1" s="43"/>
+      <c r="J1" s="43"/>
+      <c r="K1" s="43"/>
+      <c r="L1" s="43"/>
+      <c r="M1" s="43"/>
+      <c r="N1" s="43"/>
+      <c r="O1" s="43"/>
+      <c r="P1" s="43"/>
+      <c r="Q1" s="43"/>
+      <c r="R1" s="43"/>
+      <c r="S1" s="43"/>
+      <c r="T1" s="43"/>
+      <c r="U1" s="43"/>
+      <c r="V1" s="43"/>
+      <c r="W1" s="43"/>
+      <c r="X1" s="43"/>
+    </row>
+    <row r="2" spans="1:24" s="18" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="B2" s="40"/>
-      <c r="C2" s="40"/>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
-      <c r="G2" s="40"/>
-      <c r="H2" s="40"/>
-      <c r="I2" s="40"/>
-      <c r="J2" s="40"/>
-      <c r="K2" s="40"/>
-      <c r="L2" s="40"/>
-      <c r="M2" s="40"/>
-      <c r="N2" s="40"/>
-      <c r="O2" s="40"/>
-      <c r="P2" s="40"/>
-      <c r="Q2" s="40"/>
-      <c r="R2" s="40"/>
-      <c r="S2" s="40"/>
-      <c r="T2" s="40"/>
-      <c r="U2" s="40"/>
-      <c r="V2" s="40"/>
-      <c r="W2" s="40"/>
-      <c r="X2" s="40"/>
-    </row>
-    <row r="3" spans="1:24" s="3" customFormat="1" ht="10.199999999999999" x14ac:dyDescent="0.3">
+      <c r="B2" s="44"/>
+      <c r="C2" s="44"/>
+      <c r="D2" s="44"/>
+      <c r="E2" s="44"/>
+      <c r="F2" s="44"/>
+      <c r="G2" s="44"/>
+      <c r="H2" s="44"/>
+      <c r="I2" s="44"/>
+      <c r="J2" s="44"/>
+      <c r="K2" s="44"/>
+      <c r="L2" s="44"/>
+      <c r="M2" s="44"/>
+      <c r="N2" s="44"/>
+      <c r="O2" s="44"/>
+      <c r="P2" s="44"/>
+      <c r="Q2" s="44"/>
+      <c r="R2" s="44"/>
+      <c r="S2" s="44"/>
+      <c r="T2" s="44"/>
+      <c r="U2" s="44"/>
+      <c r="V2" s="44"/>
+      <c r="W2" s="44"/>
+      <c r="X2" s="44"/>
+    </row>
+    <row r="3" spans="1:24" s="3" customFormat="1" ht="10.5" x14ac:dyDescent="0.35">
       <c r="C3" s="4"/>
       <c r="I3" s="4"/>
       <c r="V3" s="4"/>
     </row>
-    <row r="4" spans="1:24" s="10" customFormat="1" ht="40.799999999999997" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:24" s="10" customFormat="1" ht="42" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>11</v>
       </c>
@@ -2124,7 +2124,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="5" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="8"/>
       <c r="B5" s="6"/>
       <c r="C5" s="6"/>
@@ -2150,7 +2150,7 @@
       <c r="W5" s="7"/>
       <c r="X5" s="7"/>
     </row>
-    <row r="6" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="13" t="s">
         <v>61</v>
       </c>
@@ -2218,7 +2218,7 @@
       </c>
       <c r="X6" s="15"/>
     </row>
-    <row r="7" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="8"/>
       <c r="B7" s="6"/>
       <c r="C7" s="6"/>
@@ -2244,7 +2244,7 @@
       <c r="W7" s="7"/>
       <c r="X7" s="7"/>
     </row>
-    <row r="8" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="13" t="s">
         <v>62</v>
       </c>
@@ -2294,7 +2294,7 @@
       </c>
       <c r="X8" s="15"/>
     </row>
-    <row r="9" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="8"/>
       <c r="B9" s="6"/>
       <c r="C9" s="6"/>
@@ -2320,7 +2320,7 @@
       <c r="W9" s="7"/>
       <c r="X9" s="7"/>
     </row>
-    <row r="10" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="13" t="s">
         <v>63</v>
       </c>
@@ -2370,7 +2370,7 @@
       </c>
       <c r="X10" s="15"/>
     </row>
-    <row r="11" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="8"/>
       <c r="B11" s="6"/>
       <c r="C11" s="6"/>
@@ -2396,7 +2396,7 @@
       <c r="W11" s="7"/>
       <c r="X11" s="7"/>
     </row>
-    <row r="12" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="13" t="s">
         <v>64</v>
       </c>
@@ -2446,7 +2446,7 @@
       </c>
       <c r="X12" s="15"/>
     </row>
-    <row r="13" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="8"/>
       <c r="B13" s="6"/>
       <c r="C13" s="6"/>
@@ -2472,7 +2472,7 @@
       <c r="W13" s="7"/>
       <c r="X13" s="7"/>
     </row>
-    <row r="14" spans="1:24" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:24" s="16" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="13" t="s">
         <v>65</v>
       </c>
@@ -2524,7 +2524,7 @@
       </c>
       <c r="X14" s="15"/>
     </row>
-    <row r="15" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:24" s="9" customFormat="1" ht="3.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="8"/>
       <c r="B15" s="6"/>
       <c r="C15" s="6"/>
@@ -2550,7 +2550,7 @@
       <c r="W15" s="7"/>
       <c r="X15" s="7"/>
     </row>
-    <row r="16" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:24" s="16" customFormat="1" ht="27" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A16" s="13" t="s">
         <v>66</v>
       </c>
@@ -2622,19 +2622,19 @@
       <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="10.199999999999999" zeroHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="0" defaultRowHeight="10.5" zeroHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.5546875" style="25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.5546875" style="27" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" style="21" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.54296875" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="37.54296875" style="27" customWidth="1"/>
+    <col min="3" max="3" width="4.90625" style="21" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8" style="21" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.453125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="15" style="22" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="3.33203125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="9.109375" style="21" hidden="1"/>
+    <col min="7" max="7" width="3.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="9.08984375" style="21" hidden="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>53</v>
       </c>
@@ -2657,7 +2657,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B2" s="3"/>
       <c r="D2" s="21" t="s">
         <v>58</v>
@@ -2672,7 +2672,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B3" s="26"/>
       <c r="D3" s="21" t="s">
         <v>56</v>
@@ -2687,7 +2687,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B4" s="26"/>
       <c r="D4" s="3"/>
       <c r="E4" s="3" t="s">
@@ -2698,7 +2698,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B5" s="26"/>
       <c r="E5" s="3" t="s">
         <v>17</v>
@@ -2707,7 +2707,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" s="3" t="s">
         <v>18</v>
       </c>
@@ -2715,7 +2715,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
@@ -2723,102 +2723,102 @@
         <v>27</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G8" s="23" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G9" s="23" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G10" s="23" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G11" s="23" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G12" s="23" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G13" s="23" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G14" s="23" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G15" s="23" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="G16" s="23" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="17" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="17" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G17" s="23" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="18" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G18" s="23" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="19" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="19" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G19" s="23" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="20" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="20" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G20" s="23" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="21" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G21" s="23" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="22" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G22" s="23" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="23" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="23" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G23" s="23" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="24" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="24" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G24" s="23" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="25" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="25" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G25" s="23" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="26" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="26" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G26" s="23" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="27" spans="7:7" x14ac:dyDescent="0.2">
+    <row r="27" spans="7:7" x14ac:dyDescent="0.25">
       <c r="G27" s="23" t="s">
         <v>47</v>
       </c>
@@ -2830,6 +2830,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x010100F70625ADBA56594DA36B3643412C2A87" ma:contentTypeVersion="8" ma:contentTypeDescription="Crie um novo documento." ma:contentTypeScope="" ma:versionID="99cbfc35c46aa4096939fe81498bcd16">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="4c250455-3b8d-490f-a74f-467a645409fe" xmlns:ns3="9e2e9b43-9c28-46fa-a19f-9ced5b973392" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4fd665cb41ca1f10e9b8659161501aa6" ns2:_="" ns3:_="">
     <xsd:import namespace="4c250455-3b8d-490f-a74f-467a645409fe"/>
@@ -3020,15 +3029,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement/>
@@ -3036,6 +3036,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{811B6344-58FA-4AAC-A4E4-919F024182C6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D156E915-3DEC-46EC-A41E-F69269F9AEE5}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -3054,14 +3062,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{811B6344-58FA-4AAC-A4E4-919F024182C6}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{52422203-45D4-4464-9FCA-30E9A184D3FD}">
   <ds:schemaRefs>

</xml_diff>